<commit_message>
Added presentation file and fixed excel file
</commit_message>
<xml_diff>
--- a/summery of datasets.xlsx
+++ b/summery of datasets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ttomn\OneDrive\Desktop\data-science-transportation-research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C8265A-FA68-44A5-B3BA-2E1664E4A9E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EACD5A41-AA55-4C03-9396-43D52AD86B9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1470" windowWidth="29040" windowHeight="15720" xr2:uid="{72263929-EDEF-4E21-B5DD-DE91C767F2F3}"/>
+    <workbookView xWindow="28680" yWindow="-15" windowWidth="29040" windowHeight="15720" xr2:uid="{72263929-EDEF-4E21-B5DD-DE91C767F2F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
   <si>
     <t>name</t>
   </si>
@@ -164,13 +164,19 @@
     <t>Accident Analysis and Prevention</t>
   </si>
   <si>
-    <t>Open Parking and Camera Violations</t>
-  </si>
-  <si>
     <t>91M+</t>
   </si>
   <si>
     <t>20.5K</t>
+  </si>
+  <si>
+    <t>42.8K</t>
+  </si>
+  <si>
+    <t>traffic volume counts</t>
+  </si>
+  <si>
+    <t>open parking and camera violations</t>
   </si>
 </sst>
 </file>
@@ -277,8 +283,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C0788ED5-C00A-468A-9463-290CE9069617}" name="Table1" displayName="Table1" ref="A1:F13" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F13" xr:uid="{C0788ED5-C00A-468A-9463-290CE9069617}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C0788ED5-C00A-468A-9463-290CE9069617}" name="Table1" displayName="Table1" ref="A1:F14" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F14" xr:uid="{C0788ED5-C00A-468A-9463-290CE9069617}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{C327A4F4-3FD8-4376-936A-CADECDE349C3}" name="name" dataDxfId="3" dataCellStyle="Hyperlink"/>
     <tableColumn id="2" xr3:uid="{CE689B43-2486-40DC-B4C5-8476D7A53B1C}" name="start date"/>
@@ -588,15 +594,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1BDF10A-F706-42C4-9C77-6FC57452C037}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="23.09765625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="32.69921875" style="5" customWidth="1"/>
+    <col min="2" max="3" width="13.3984375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="17.796875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="17.59765625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="23.09765625" style="5" customWidth="1"/>
     <col min="7" max="16384" width="8.796875" style="5"/>
   </cols>
   <sheetData>
@@ -640,100 +650,98 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B3" s="4">
-        <v>35072</v>
+        <v>44562</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E3" s="2">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B4" s="4">
-        <v>41831</v>
-      </c>
-      <c r="C4" s="4">
-        <v>41831</v>
+        <v>43101</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="E4" s="2">
-        <v>6</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>12</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="4">
-        <v>44562</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>31</v>
+      <c r="A5" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="7">
+        <v>36526</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="E5" s="2">
-        <v>14</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>15</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4">
-        <v>43101</v>
+        <v>35072</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="E6" s="2">
-        <v>13</v>
-      </c>
-      <c r="F6" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="B7" s="4">
+        <v>41831</v>
+      </c>
+      <c r="C7" s="4">
+        <v>41831</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="E7" s="2">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -815,59 +823,79 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="7">
+        <v>41122</v>
+      </c>
+      <c r="C12" s="7">
+        <v>44325</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="2">
+        <v>31</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="2">
+        <v>16</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="D12" s="5" t="s">
+      <c r="B14" s="7"/>
+      <c r="D14" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E14" s="2">
         <v>30</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="7">
-        <v>36526</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" s="2">
-        <v>19</v>
-      </c>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
         <v>41</v>
       </c>
     </row>
@@ -875,27 +903,28 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="https://data.cityofnewyork.us/Public-Safety/Motor-Vehicle-Collisions-Crashes/h9gi-nx95" xr:uid="{079D6C61-1F3E-47D1-8A72-2C071EC46887}"/>
-    <hyperlink ref="A3" r:id="rId2" display="https://data.cityofnewyork.us/Transportation/VZV_Speed-Humps/7f9e-jic4" xr:uid="{684E0E2B-4BC6-4C74-8101-F9125CC6B4DB}"/>
-    <hyperlink ref="A4" r:id="rId3" display="https://data.cityofnewyork.us/Transportation/VZV_Speed-Limits/7n5j-865y" xr:uid="{9C7C46EF-F6C5-4493-8D55-9551B75460A2}"/>
-    <hyperlink ref="A5" r:id="rId4" display="https://data.cityofnewyork.us/Public-Safety/NYPD-B-Summons-Year-to-Date-/57p3-pdcj" xr:uid="{62681803-2A2C-4CA3-BD38-8D460845F4E5}"/>
-    <hyperlink ref="A6" r:id="rId5" display="https://data.cityofnewyork.us/Public-Safety/NYPD-B-Summons-Historic-/bme5-7ty4" xr:uid="{69109D88-E972-4EED-898C-E9DE47A74E02}"/>
-    <hyperlink ref="A7" r:id="rId6" xr:uid="{84473FBA-EC7D-45F5-9B46-22C6BF95640F}"/>
+    <hyperlink ref="A6" r:id="rId2" display="https://data.cityofnewyork.us/Transportation/VZV_Speed-Humps/7f9e-jic4" xr:uid="{684E0E2B-4BC6-4C74-8101-F9125CC6B4DB}"/>
+    <hyperlink ref="A7" r:id="rId3" display="https://data.cityofnewyork.us/Transportation/VZV_Speed-Limits/7n5j-865y" xr:uid="{9C7C46EF-F6C5-4493-8D55-9551B75460A2}"/>
+    <hyperlink ref="A3" r:id="rId4" display="https://data.cityofnewyork.us/Public-Safety/NYPD-B-Summons-Year-to-Date-/57p3-pdcj" xr:uid="{62681803-2A2C-4CA3-BD38-8D460845F4E5}"/>
+    <hyperlink ref="A4" r:id="rId5" display="https://data.cityofnewyork.us/Public-Safety/NYPD-B-Summons-Historic-/bme5-7ty4" xr:uid="{69109D88-E972-4EED-898C-E9DE47A74E02}"/>
+    <hyperlink ref="A13" r:id="rId6" xr:uid="{84473FBA-EC7D-45F5-9B46-22C6BF95640F}"/>
     <hyperlink ref="A8" r:id="rId7" xr:uid="{85A1CF57-611A-4653-8CD6-9BDC199621E4}"/>
     <hyperlink ref="A9" r:id="rId8" xr:uid="{5DA29884-7A78-428B-8070-E6DAB4DF13E6}"/>
     <hyperlink ref="A10" r:id="rId9" xr:uid="{4823D81B-30CE-4D82-AABA-05FB8D03C095}"/>
     <hyperlink ref="A11" r:id="rId10" xr:uid="{37A35CC4-1BB6-43C0-8719-37647D9A1C33}"/>
-    <hyperlink ref="A15" r:id="rId11" xr:uid="{9BD2C229-7ED8-42CF-9106-1C96E149C0F1}"/>
-    <hyperlink ref="A16" r:id="rId12" xr:uid="{6F2A14F2-811D-49F1-B327-0E176A835FBC}"/>
-    <hyperlink ref="A17" r:id="rId13" xr:uid="{7982FCFD-1A33-46AE-A6E9-794818E0D566}"/>
-    <hyperlink ref="A18" r:id="rId14" xr:uid="{C5E884F6-EF04-4712-8CB8-3A1BA22DFBB3}"/>
-    <hyperlink ref="A12" r:id="rId15" xr:uid="{4107B053-7C68-42A7-9165-4B339FA24096}"/>
-    <hyperlink ref="A19" r:id="rId16" xr:uid="{D582DBF5-F05F-4408-8F9A-5FBCC2B20E62}"/>
-    <hyperlink ref="A13" r:id="rId17" xr:uid="{CDBE651B-B9D5-4C4D-B0EF-B25302EAB387}"/>
+    <hyperlink ref="A16" r:id="rId11" xr:uid="{9BD2C229-7ED8-42CF-9106-1C96E149C0F1}"/>
+    <hyperlink ref="A17" r:id="rId12" xr:uid="{6F2A14F2-811D-49F1-B327-0E176A835FBC}"/>
+    <hyperlink ref="A18" r:id="rId13" xr:uid="{7982FCFD-1A33-46AE-A6E9-794818E0D566}"/>
+    <hyperlink ref="A19" r:id="rId14" xr:uid="{C5E884F6-EF04-4712-8CB8-3A1BA22DFBB3}"/>
+    <hyperlink ref="A20" r:id="rId15" xr:uid="{D582DBF5-F05F-4408-8F9A-5FBCC2B20E62}"/>
+    <hyperlink ref="A5" r:id="rId16" display="Open Parking and Camera Violations" xr:uid="{CDBE651B-B9D5-4C4D-B0EF-B25302EAB387}"/>
+    <hyperlink ref="A12" r:id="rId17" display="Traffic Volume Counts" xr:uid="{5D2D375A-7E9C-4E79-9C4F-35B4CD4411F5}"/>
+    <hyperlink ref="A14" r:id="rId18" xr:uid="{20498583-301B-47C0-9249-D0035F8E5C8C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId18"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId19"/>
   <tableParts count="1">
-    <tablePart r:id="rId19"/>
+    <tablePart r:id="rId20"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>